<commit_message>
add extra fake courses
</commit_message>
<xml_diff>
--- a/course_schedules.xlsx
+++ b/course_schedules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="121">
   <si>
     <t>序号</t>
   </si>
@@ -369,13 +369,38 @@
   </si>
   <si>
     <t>周其仁</t>
+  </si>
+  <si>
+    <t>我只是来求课的TvT</t>
+  </si>
+  <si>
+    <t>我是雷锋我就是来出课的</t>
+  </si>
+  <si>
+    <t>无</t>
+    <rPh sb="0" eb="1">
+      <t>wu</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>理教666</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1--12</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1--12</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -404,6 +429,24 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
@@ -479,8 +522,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -512,8 +561,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -788,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33:N33"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -2374,8 +2429,81 @@
       </c>
       <c r="P46" s="5"/>
     </row>
+    <row r="47" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>31</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E47" s="5">
+        <v>2</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="P47" s="5"/>
+    </row>
+    <row r="48" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>32</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E48" s="5">
+        <v>2</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="P48" s="5"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
clear option needs password & delete fake courses
</commit_message>
<xml_diff>
--- a/course_schedules.xlsx
+++ b/course_schedules.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -16,6 +16,9 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="115">
   <si>
     <t>序号</t>
   </si>
@@ -369,31 +372,6 @@
   </si>
   <si>
     <t>周其仁</t>
-  </si>
-  <si>
-    <t>我只是来求课的TvT</t>
-  </si>
-  <si>
-    <t>我是雷锋我就是来出课的</t>
-  </si>
-  <si>
-    <t>无</t>
-    <rPh sb="0" eb="1">
-      <t>wu</t>
-    </rPh>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>理教666</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1--12</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1--12</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -846,7 +824,7 @@
   <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+      <selection activeCell="R40" sqref="R40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -2430,75 +2408,39 @@
       <c r="P46" s="5"/>
     </row>
     <row r="47" spans="1:16" ht="17" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
-        <v>31</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E47" s="5">
-        <v>2</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>120</v>
-      </c>
+      <c r="A47" s="4"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
       <c r="M47" s="5"/>
       <c r="N47" s="5"/>
-      <c r="O47" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="O47" s="5"/>
       <c r="P47" s="5"/>
     </row>
     <row r="48" spans="1:16" ht="17" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
-        <v>32</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E48" s="5">
-        <v>2</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>119</v>
-      </c>
+      <c r="A48" s="4"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
       <c r="N48" s="5"/>
-      <c r="O48" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="O48" s="5"/>
       <c r="P48" s="5"/>
     </row>
   </sheetData>

</xml_diff>